<commit_message>
breakpoint feature eng pt 1
</commit_message>
<xml_diff>
--- a/data/breakpoint_data.xlsx
+++ b/data/breakpoint_data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="142">
   <si>
     <t>Player</t>
   </si>
@@ -185,7 +185,7 @@
     <t>aBeZy</t>
   </si>
   <si>
-    <t>Lynz</t>
+    <t>Lyynnz</t>
   </si>
   <si>
     <t>Nero</t>
@@ -350,6 +350,24 @@
     <t>#</t>
   </si>
   <si>
+    <t>Total_Series_Wins</t>
+  </si>
+  <si>
+    <t>Total_Series_Losses</t>
+  </si>
+  <si>
+    <t>Total_Series %</t>
+  </si>
+  <si>
+    <t>Total_Map_Wins</t>
+  </si>
+  <si>
+    <t>Total_Map_Losses</t>
+  </si>
+  <si>
+    <t>Total_Maps %</t>
+  </si>
+  <si>
     <t>HP +/-</t>
   </si>
   <si>
@@ -473,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -505,6 +523,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="10" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -2478,7 +2499,7 @@
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="6" t="s">
         <v>57</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -5146,7 +5167,7 @@
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="9" t="s">
         <v>89</v>
       </c>
       <c r="B49" s="6" t="s">
@@ -13635,7 +13656,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="30" width="10.56"/>
+    <col customWidth="1" min="1" max="36" width="10.56"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -13645,38 +13666,38 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>121</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>122</v>
@@ -13684,65 +13705,95 @@
       <c r="O1" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="V1" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="F2" s="8">
+        <v>13.0</v>
+      </c>
+      <c r="G2" s="8">
+        <v>8.0</v>
+      </c>
+      <c r="H2" s="8">
+        <v>0.619</v>
+      </c>
+      <c r="I2" s="7">
         <v>38.9</v>
       </c>
-      <c r="D2" s="14">
+      <c r="J2" s="14">
         <v>0.7</v>
       </c>
-      <c r="E2" s="7">
+      <c r="K2" s="7">
         <v>1.05</v>
       </c>
-      <c r="F2" s="7">
+      <c r="L2" s="7">
         <v>234.7</v>
-      </c>
-      <c r="G2" s="7">
-        <v>1.04</v>
-      </c>
-      <c r="H2" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="I2" s="7">
-        <v>0.96</v>
-      </c>
-      <c r="J2" s="7">
-        <v>4.33</v>
-      </c>
-      <c r="K2" s="7">
-        <v>-0.67</v>
-      </c>
-      <c r="L2" s="14">
-        <v>0.6</v>
       </c>
       <c r="M2" s="7">
         <v>1.04</v>
       </c>
-      <c r="N2" s="7">
+      <c r="N2" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="O2" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="P2" s="7">
+        <v>4.33</v>
+      </c>
+      <c r="Q2" s="7">
+        <v>-0.67</v>
+      </c>
+      <c r="R2" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="S2" s="7">
+        <v>1.04</v>
+      </c>
+      <c r="T2" s="7">
         <v>2.4</v>
       </c>
-      <c r="O2" s="7">
+      <c r="U2" s="7">
         <v>0.2</v>
       </c>
-      <c r="P2" s="8">
+      <c r="V2" s="8">
         <v>2025.0</v>
       </c>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13"/>
       <c r="W2" s="13"/>
       <c r="X2" s="13"/>
       <c r="Y2" s="13"/>
@@ -13751,62 +13802,80 @@
       <c r="AB2" s="13"/>
       <c r="AC2" s="13"/>
       <c r="AD2" s="13"/>
+      <c r="AE2" s="13"/>
+      <c r="AF2" s="13"/>
+      <c r="AG2" s="13"/>
+      <c r="AH2" s="13"/>
+      <c r="AI2" s="13"/>
+      <c r="AJ2" s="13"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="D3" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0.714</v>
+      </c>
+      <c r="F3" s="8">
+        <v>19.0</v>
+      </c>
+      <c r="G3" s="8">
+        <v>11.0</v>
+      </c>
+      <c r="H3" s="8">
+        <v>0.633</v>
+      </c>
+      <c r="I3" s="7">
         <v>33.33</v>
       </c>
-      <c r="D3" s="14">
+      <c r="J3" s="14">
         <v>0.583</v>
       </c>
-      <c r="E3" s="7">
+      <c r="K3" s="7">
         <v>1.1</v>
       </c>
-      <c r="F3" s="7">
+      <c r="L3" s="7">
         <v>231.08</v>
       </c>
-      <c r="G3" s="7">
+      <c r="M3" s="7">
         <v>1.08</v>
       </c>
-      <c r="H3" s="14">
+      <c r="N3" s="14">
         <v>0.636</v>
       </c>
-      <c r="I3" s="7">
+      <c r="O3" s="7">
         <v>1.06</v>
       </c>
-      <c r="J3" s="7">
+      <c r="P3" s="7">
         <v>5.0</v>
       </c>
-      <c r="K3" s="7">
+      <c r="Q3" s="7">
         <v>0.64</v>
       </c>
-      <c r="L3" s="14">
+      <c r="R3" s="14">
         <v>0.714</v>
       </c>
-      <c r="M3" s="7">
+      <c r="S3" s="7">
         <v>1.06</v>
       </c>
-      <c r="N3" s="7">
+      <c r="T3" s="7">
         <v>2.43</v>
       </c>
-      <c r="O3" s="7">
+      <c r="U3" s="7">
         <v>1.0</v>
       </c>
-      <c r="P3" s="8">
+      <c r="V3" s="8">
         <v>2025.0</v>
       </c>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
-      <c r="V3" s="13"/>
       <c r="W3" s="13"/>
       <c r="X3" s="13"/>
       <c r="Y3" s="13"/>
@@ -13815,62 +13884,80 @@
       <c r="AB3" s="13"/>
       <c r="AC3" s="13"/>
       <c r="AD3" s="13"/>
+      <c r="AE3" s="13"/>
+      <c r="AF3" s="13"/>
+      <c r="AG3" s="13"/>
+      <c r="AH3" s="13"/>
+      <c r="AI3" s="13"/>
+      <c r="AJ3" s="13"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="11">
+        <v>5.0</v>
+      </c>
+      <c r="D4" s="11">
+        <v>3.0</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0.625</v>
+      </c>
+      <c r="F4" s="11">
+        <v>18.0</v>
+      </c>
+      <c r="G4" s="11">
+        <v>15.0</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0.545</v>
+      </c>
+      <c r="I4" s="7">
         <v>29.2</v>
       </c>
-      <c r="D4" s="14">
+      <c r="J4" s="14">
         <v>0.733</v>
       </c>
-      <c r="E4" s="7">
+      <c r="K4" s="7">
         <v>1.1</v>
       </c>
-      <c r="F4" s="7">
+      <c r="L4" s="7">
         <v>213.73</v>
       </c>
-      <c r="G4" s="7">
+      <c r="M4" s="7">
         <v>1.04</v>
       </c>
-      <c r="H4" s="14">
+      <c r="N4" s="14">
         <v>0.5</v>
       </c>
-      <c r="I4" s="7">
+      <c r="O4" s="7">
         <v>1.02</v>
       </c>
-      <c r="J4" s="7">
+      <c r="P4" s="7">
         <v>4.9</v>
       </c>
-      <c r="K4" s="7">
+      <c r="Q4" s="7">
         <v>0.4</v>
       </c>
-      <c r="L4" s="14">
+      <c r="R4" s="14">
         <v>0.25</v>
       </c>
-      <c r="M4" s="7">
+      <c r="S4" s="7">
         <v>0.95</v>
       </c>
-      <c r="N4" s="7">
+      <c r="T4" s="7">
         <v>2.13</v>
       </c>
-      <c r="O4" s="7">
+      <c r="U4" s="7">
         <v>-0.63</v>
       </c>
-      <c r="P4" s="8">
+      <c r="V4" s="8">
         <v>2025.0</v>
       </c>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
-      <c r="V4" s="13"/>
       <c r="W4" s="13"/>
       <c r="X4" s="13"/>
       <c r="Y4" s="13"/>
@@ -13879,62 +13966,80 @@
       <c r="AB4" s="13"/>
       <c r="AC4" s="13"/>
       <c r="AD4" s="13"/>
+      <c r="AE4" s="13"/>
+      <c r="AF4" s="13"/>
+      <c r="AG4" s="13"/>
+      <c r="AH4" s="13"/>
+      <c r="AI4" s="13"/>
+      <c r="AJ4" s="13"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="8">
+        <v>6.0</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0.857</v>
+      </c>
+      <c r="F5" s="8">
+        <v>19.0</v>
+      </c>
+      <c r="G5" s="8">
+        <v>11.0</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0.633</v>
+      </c>
+      <c r="I5" s="7">
         <v>17.46</v>
       </c>
-      <c r="D5" s="14">
+      <c r="J5" s="14">
         <v>0.538</v>
       </c>
-      <c r="E5" s="7">
+      <c r="K5" s="7">
         <v>1.03</v>
       </c>
-      <c r="F5" s="7">
+      <c r="L5" s="7">
         <v>218.62</v>
       </c>
-      <c r="G5" s="7">
+      <c r="M5" s="7">
         <v>1.03</v>
       </c>
-      <c r="H5" s="14">
+      <c r="N5" s="14">
         <v>0.7</v>
       </c>
-      <c r="I5" s="7">
+      <c r="O5" s="7">
         <v>1.04</v>
       </c>
-      <c r="J5" s="7">
+      <c r="P5" s="7">
         <v>5.1</v>
       </c>
-      <c r="K5" s="7">
+      <c r="Q5" s="7">
         <v>1.0</v>
       </c>
-      <c r="L5" s="14">
+      <c r="R5" s="14">
         <v>0.714</v>
       </c>
-      <c r="M5" s="7">
+      <c r="S5" s="7">
         <v>1.05</v>
       </c>
-      <c r="N5" s="7">
+      <c r="T5" s="7">
         <v>2.43</v>
       </c>
-      <c r="O5" s="7">
+      <c r="U5" s="7">
         <v>0.57</v>
       </c>
-      <c r="P5" s="8">
+      <c r="V5" s="8">
         <v>2025.0</v>
       </c>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
       <c r="W5" s="13"/>
       <c r="X5" s="13"/>
       <c r="Y5" s="13"/>
@@ -13943,62 +14048,80 @@
       <c r="AB5" s="13"/>
       <c r="AC5" s="13"/>
       <c r="AD5" s="13"/>
+      <c r="AE5" s="13"/>
+      <c r="AF5" s="13"/>
+      <c r="AG5" s="13"/>
+      <c r="AH5" s="13"/>
+      <c r="AI5" s="13"/>
+      <c r="AJ5" s="13"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="D6" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="F6" s="8">
+        <v>13.0</v>
+      </c>
+      <c r="G6" s="8">
+        <v>12.0</v>
+      </c>
+      <c r="H6" s="8">
+        <v>0.52</v>
+      </c>
+      <c r="I6" s="7">
         <v>12.4</v>
       </c>
-      <c r="D6" s="14">
+      <c r="J6" s="14">
         <v>0.6</v>
       </c>
-      <c r="E6" s="7">
+      <c r="K6" s="7">
         <v>1.01</v>
       </c>
-      <c r="F6" s="7">
+      <c r="L6" s="7">
         <v>227.6</v>
       </c>
-      <c r="G6" s="7">
+      <c r="M6" s="7">
         <v>1.01</v>
       </c>
-      <c r="H6" s="14">
+      <c r="N6" s="14">
         <v>0.5</v>
       </c>
-      <c r="I6" s="7">
+      <c r="O6" s="7">
         <v>1.05</v>
       </c>
-      <c r="J6" s="7">
+      <c r="P6" s="7">
         <v>5.0</v>
       </c>
-      <c r="K6" s="7">
+      <c r="Q6" s="7">
         <v>0.7</v>
       </c>
-      <c r="L6" s="14">
+      <c r="R6" s="14">
         <v>0.4</v>
       </c>
-      <c r="M6" s="7">
+      <c r="S6" s="7">
         <v>0.97</v>
       </c>
-      <c r="N6" s="7">
+      <c r="T6" s="7">
         <v>1.6</v>
       </c>
-      <c r="O6" s="7">
+      <c r="U6" s="7">
         <v>-0.2</v>
       </c>
-      <c r="P6" s="8">
+      <c r="V6" s="8">
         <v>2025.0</v>
       </c>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="13"/>
-      <c r="V6" s="13"/>
       <c r="W6" s="13"/>
       <c r="X6" s="13"/>
       <c r="Y6" s="13"/>
@@ -14007,62 +14130,80 @@
       <c r="AB6" s="13"/>
       <c r="AC6" s="13"/>
       <c r="AD6" s="13"/>
+      <c r="AE6" s="13"/>
+      <c r="AF6" s="13"/>
+      <c r="AG6" s="13"/>
+      <c r="AH6" s="13"/>
+      <c r="AI6" s="13"/>
+      <c r="AJ6" s="13"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="11">
+        <v>4.0</v>
+      </c>
+      <c r="D7" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="F7" s="11">
+        <v>14.0</v>
+      </c>
+      <c r="G7" s="11">
+        <v>8.0</v>
+      </c>
+      <c r="H7" s="11">
+        <v>0.636</v>
+      </c>
+      <c r="I7" s="7">
         <v>1.33</v>
       </c>
-      <c r="D7" s="14">
+      <c r="J7" s="14">
         <v>0.556</v>
       </c>
-      <c r="E7" s="7">
+      <c r="K7" s="7">
         <v>0.99</v>
       </c>
-      <c r="F7" s="7">
+      <c r="L7" s="7">
         <v>218.0</v>
       </c>
-      <c r="G7" s="7">
+      <c r="M7" s="7">
         <v>1.04</v>
       </c>
-      <c r="H7" s="14">
+      <c r="N7" s="14">
         <v>0.875</v>
       </c>
-      <c r="I7" s="7">
+      <c r="O7" s="7">
         <v>1.27</v>
       </c>
-      <c r="J7" s="7">
+      <c r="P7" s="7">
         <v>5.63</v>
       </c>
-      <c r="K7" s="7">
+      <c r="Q7" s="7">
         <v>2.5</v>
       </c>
-      <c r="L7" s="14">
+      <c r="R7" s="14">
         <v>0.4</v>
       </c>
-      <c r="M7" s="7">
+      <c r="S7" s="7">
         <v>1.05</v>
       </c>
-      <c r="N7" s="7">
+      <c r="T7" s="7">
         <v>2.0</v>
       </c>
-      <c r="O7" s="7">
+      <c r="U7" s="7">
         <v>-0.2</v>
       </c>
-      <c r="P7" s="8">
+      <c r="V7" s="8">
         <v>2025.0</v>
       </c>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13"/>
       <c r="W7" s="13"/>
       <c r="X7" s="13"/>
       <c r="Y7" s="13"/>
@@ -14071,62 +14212,80 @@
       <c r="AB7" s="13"/>
       <c r="AC7" s="13"/>
       <c r="AD7" s="13"/>
+      <c r="AE7" s="13"/>
+      <c r="AF7" s="13"/>
+      <c r="AG7" s="13"/>
+      <c r="AH7" s="13"/>
+      <c r="AI7" s="13"/>
+      <c r="AJ7" s="13"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="D8" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F8" s="8">
+        <v>10.0</v>
+      </c>
+      <c r="G8" s="8">
+        <v>12.0</v>
+      </c>
+      <c r="H8" s="8">
+        <v>0.454</v>
+      </c>
+      <c r="I8" s="7">
         <v>-1.44</v>
       </c>
-      <c r="D8" s="14">
+      <c r="J8" s="14">
         <v>0.556</v>
       </c>
-      <c r="E8" s="7">
+      <c r="K8" s="7">
         <v>0.99</v>
       </c>
-      <c r="F8" s="7">
+      <c r="L8" s="7">
         <v>219.33</v>
       </c>
-      <c r="G8" s="7">
+      <c r="M8" s="7">
         <v>0.99</v>
       </c>
-      <c r="H8" s="14">
+      <c r="N8" s="14">
         <v>0.125</v>
       </c>
-      <c r="I8" s="7">
+      <c r="O8" s="7">
         <v>0.83</v>
       </c>
-      <c r="J8" s="7">
+      <c r="P8" s="7">
         <v>3.0</v>
       </c>
-      <c r="K8" s="7">
+      <c r="Q8" s="7">
         <v>-2.63</v>
       </c>
-      <c r="L8" s="14">
+      <c r="R8" s="14">
         <v>0.8</v>
       </c>
-      <c r="M8" s="7">
+      <c r="S8" s="7">
         <v>1.08</v>
       </c>
-      <c r="N8" s="7">
+      <c r="T8" s="7">
         <v>2.8</v>
       </c>
-      <c r="O8" s="7">
+      <c r="U8" s="7">
         <v>1.6</v>
       </c>
-      <c r="P8" s="8">
+      <c r="V8" s="8">
         <v>2025.0</v>
       </c>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="13"/>
-      <c r="V8" s="13"/>
       <c r="W8" s="13"/>
       <c r="X8" s="13"/>
       <c r="Y8" s="13"/>
@@ -14135,62 +14294,80 @@
       <c r="AB8" s="13"/>
       <c r="AC8" s="13"/>
       <c r="AD8" s="13"/>
+      <c r="AE8" s="13"/>
+      <c r="AF8" s="13"/>
+      <c r="AG8" s="13"/>
+      <c r="AH8" s="13"/>
+      <c r="AI8" s="13"/>
+      <c r="AJ8" s="13"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="D9" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="F9" s="8">
+        <v>8.0</v>
+      </c>
+      <c r="G9" s="8">
+        <v>15.0</v>
+      </c>
+      <c r="H9" s="8">
+        <v>0.348</v>
+      </c>
+      <c r="I9" s="7">
         <v>-11.7</v>
       </c>
-      <c r="D9" s="14">
+      <c r="J9" s="14">
         <v>0.3</v>
       </c>
-      <c r="E9" s="7">
+      <c r="K9" s="7">
         <v>0.99</v>
       </c>
-      <c r="F9" s="7">
+      <c r="L9" s="7">
         <v>221.1</v>
       </c>
-      <c r="G9" s="7">
+      <c r="M9" s="7">
         <v>0.99</v>
       </c>
-      <c r="H9" s="14">
+      <c r="N9" s="14">
         <v>0.25</v>
       </c>
-      <c r="I9" s="7">
+      <c r="O9" s="7">
         <v>0.95</v>
       </c>
-      <c r="J9" s="7">
+      <c r="P9" s="7">
         <v>3.88</v>
       </c>
-      <c r="K9" s="7">
+      <c r="Q9" s="7">
         <v>-1.38</v>
       </c>
-      <c r="L9" s="14">
+      <c r="R9" s="14">
         <v>0.6</v>
       </c>
-      <c r="M9" s="7">
+      <c r="S9" s="7">
         <v>1.0</v>
       </c>
-      <c r="N9" s="7">
+      <c r="T9" s="7">
         <v>2.2</v>
       </c>
-      <c r="O9" s="7">
+      <c r="U9" s="7">
         <v>0.2</v>
       </c>
-      <c r="P9" s="8">
+      <c r="V9" s="8">
         <v>2025.0</v>
       </c>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="13"/>
-      <c r="T9" s="13"/>
-      <c r="U9" s="13"/>
-      <c r="V9" s="13"/>
       <c r="W9" s="13"/>
       <c r="X9" s="13"/>
       <c r="Y9" s="13"/>
@@ -14199,62 +14376,80 @@
       <c r="AB9" s="13"/>
       <c r="AC9" s="13"/>
       <c r="AD9" s="13"/>
+      <c r="AE9" s="13"/>
+      <c r="AF9" s="13"/>
+      <c r="AG9" s="13"/>
+      <c r="AH9" s="13"/>
+      <c r="AI9" s="13"/>
+      <c r="AJ9" s="13"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="7" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="D10" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0.333</v>
+      </c>
+      <c r="F10" s="8">
+        <v>11.0</v>
+      </c>
+      <c r="G10" s="8">
+        <v>13.0</v>
+      </c>
+      <c r="H10" s="8">
+        <v>0.458</v>
+      </c>
+      <c r="I10" s="7">
         <v>-22.9</v>
       </c>
-      <c r="D10" s="14">
+      <c r="J10" s="14">
         <v>0.6</v>
       </c>
-      <c r="E10" s="7">
+      <c r="K10" s="7">
         <v>0.95</v>
       </c>
-      <c r="F10" s="7">
+      <c r="L10" s="7">
         <v>195.7</v>
       </c>
-      <c r="G10" s="7">
+      <c r="M10" s="7">
         <v>0.92</v>
       </c>
-      <c r="H10" s="14">
+      <c r="N10" s="14">
         <v>0.5</v>
       </c>
-      <c r="I10" s="7">
+      <c r="O10" s="7">
         <v>0.97</v>
       </c>
-      <c r="J10" s="7">
+      <c r="P10" s="7">
         <v>4.63</v>
       </c>
-      <c r="K10" s="7">
+      <c r="Q10" s="7">
         <v>-0.5</v>
       </c>
-      <c r="L10" s="14">
+      <c r="R10" s="14">
         <v>0.167</v>
       </c>
-      <c r="M10" s="7">
+      <c r="S10" s="7">
         <v>0.86</v>
       </c>
-      <c r="N10" s="7">
+      <c r="T10" s="7">
         <v>1.33</v>
       </c>
-      <c r="O10" s="7">
+      <c r="U10" s="7">
         <v>-1.33</v>
       </c>
-      <c r="P10" s="8">
+      <c r="V10" s="8">
         <v>2025.0</v>
       </c>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="13"/>
-      <c r="V10" s="13"/>
       <c r="W10" s="13"/>
       <c r="X10" s="13"/>
       <c r="Y10" s="13"/>
@@ -14263,62 +14458,80 @@
       <c r="AB10" s="13"/>
       <c r="AC10" s="13"/>
       <c r="AD10" s="13"/>
+      <c r="AE10" s="13"/>
+      <c r="AF10" s="13"/>
+      <c r="AG10" s="13"/>
+      <c r="AH10" s="13"/>
+      <c r="AI10" s="13"/>
+      <c r="AJ10" s="13"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="7" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="D11" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="E11" s="8">
+        <v>57.1</v>
+      </c>
+      <c r="F11" s="8">
+        <v>16.0</v>
+      </c>
+      <c r="G11" s="8">
+        <v>17.0</v>
+      </c>
+      <c r="H11" s="8">
+        <v>0.485</v>
+      </c>
+      <c r="I11" s="7">
         <v>-23.21</v>
       </c>
-      <c r="D11" s="14">
+      <c r="J11" s="14">
         <v>0.286</v>
       </c>
-      <c r="E11" s="7">
+      <c r="K11" s="7">
         <v>0.96</v>
       </c>
-      <c r="F11" s="7">
+      <c r="L11" s="7">
         <v>216.07</v>
       </c>
-      <c r="G11" s="7">
+      <c r="M11" s="7">
         <v>0.98</v>
       </c>
-      <c r="H11" s="14">
+      <c r="N11" s="14">
         <v>0.583</v>
       </c>
-      <c r="I11" s="7">
+      <c r="O11" s="7">
         <v>1.0</v>
       </c>
-      <c r="J11" s="7">
+      <c r="P11" s="7">
         <v>4.67</v>
       </c>
-      <c r="K11" s="7">
+      <c r="Q11" s="7">
         <v>0.17</v>
       </c>
-      <c r="L11" s="14">
+      <c r="R11" s="14">
         <v>0.714</v>
       </c>
-      <c r="M11" s="7">
+      <c r="S11" s="7">
         <v>1.02</v>
       </c>
-      <c r="N11" s="7">
+      <c r="T11" s="7">
         <v>2.43</v>
       </c>
-      <c r="O11" s="7">
+      <c r="U11" s="7">
         <v>0.71</v>
       </c>
-      <c r="P11" s="8">
+      <c r="V11" s="8">
         <v>2025.0</v>
       </c>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13"/>
-      <c r="T11" s="13"/>
-      <c r="U11" s="13"/>
-      <c r="V11" s="13"/>
       <c r="W11" s="13"/>
       <c r="X11" s="13"/>
       <c r="Y11" s="13"/>
@@ -14327,62 +14540,80 @@
       <c r="AB11" s="13"/>
       <c r="AC11" s="13"/>
       <c r="AD11" s="13"/>
+      <c r="AE11" s="13"/>
+      <c r="AF11" s="13"/>
+      <c r="AG11" s="13"/>
+      <c r="AH11" s="13"/>
+      <c r="AI11" s="13"/>
+      <c r="AJ11" s="13"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="7" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="D12" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F12" s="8">
+        <v>8.0</v>
+      </c>
+      <c r="G12" s="8">
+        <v>14.0</v>
+      </c>
+      <c r="H12" s="8">
+        <v>0.364</v>
+      </c>
+      <c r="I12" s="7">
         <v>-48.78</v>
       </c>
-      <c r="D12" s="14">
+      <c r="J12" s="14">
         <v>0.333</v>
       </c>
-      <c r="E12" s="7">
+      <c r="K12" s="7">
         <v>0.88</v>
       </c>
-      <c r="F12" s="7">
+      <c r="L12" s="7">
         <v>185.78</v>
       </c>
-      <c r="G12" s="7">
+      <c r="M12" s="7">
         <v>0.91</v>
       </c>
-      <c r="H12" s="14">
+      <c r="N12" s="14">
         <v>0.375</v>
       </c>
-      <c r="I12" s="7">
+      <c r="O12" s="7">
         <v>0.88</v>
       </c>
-      <c r="J12" s="7">
+      <c r="P12" s="7">
         <v>4.5</v>
       </c>
-      <c r="K12" s="7">
+      <c r="Q12" s="7">
         <v>-0.63</v>
       </c>
-      <c r="L12" s="14">
+      <c r="R12" s="14">
         <v>0.4</v>
       </c>
-      <c r="M12" s="7">
+      <c r="S12" s="7">
         <v>1.0</v>
       </c>
-      <c r="N12" s="7">
+      <c r="T12" s="7">
         <v>1.6</v>
       </c>
-      <c r="O12" s="7">
+      <c r="U12" s="7">
         <v>-0.4</v>
       </c>
-      <c r="P12" s="8">
+      <c r="V12" s="8">
         <v>2025.0</v>
       </c>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="13"/>
-      <c r="S12" s="13"/>
-      <c r="T12" s="13"/>
-      <c r="U12" s="13"/>
-      <c r="V12" s="13"/>
       <c r="W12" s="13"/>
       <c r="X12" s="13"/>
       <c r="Y12" s="13"/>
@@ -14391,62 +14622,80 @@
       <c r="AB12" s="13"/>
       <c r="AC12" s="13"/>
       <c r="AD12" s="13"/>
+      <c r="AE12" s="13"/>
+      <c r="AF12" s="13"/>
+      <c r="AG12" s="13"/>
+      <c r="AH12" s="13"/>
+      <c r="AI12" s="13"/>
+      <c r="AJ12" s="13"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="7" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="D13" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="F13" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="G13" s="8">
+        <v>15.0</v>
+      </c>
+      <c r="H13" s="8">
+        <v>0.118</v>
+      </c>
+      <c r="I13" s="7">
         <v>-66.71</v>
       </c>
-      <c r="D13" s="14">
+      <c r="J13" s="14">
         <v>0.0</v>
       </c>
-      <c r="E13" s="7">
+      <c r="K13" s="7">
         <v>0.89</v>
       </c>
-      <c r="F13" s="7">
+      <c r="L13" s="7">
         <v>183.29</v>
       </c>
-      <c r="G13" s="7">
+      <c r="M13" s="7">
         <v>0.9</v>
       </c>
-      <c r="H13" s="14">
+      <c r="N13" s="14">
         <v>0.2</v>
       </c>
-      <c r="I13" s="7">
+      <c r="O13" s="7">
         <v>0.9</v>
       </c>
-      <c r="J13" s="7">
+      <c r="P13" s="7">
         <v>4.2</v>
       </c>
-      <c r="K13" s="7">
+      <c r="Q13" s="7">
         <v>-1.0</v>
       </c>
-      <c r="L13" s="14">
+      <c r="R13" s="14">
         <v>0.2</v>
       </c>
-      <c r="M13" s="7">
+      <c r="S13" s="7">
         <v>0.93</v>
       </c>
-      <c r="N13" s="7">
+      <c r="T13" s="7">
         <v>1.0</v>
       </c>
-      <c r="O13" s="7">
+      <c r="U13" s="7">
         <v>-1.8</v>
       </c>
-      <c r="P13" s="8">
+      <c r="V13" s="8">
         <v>2025.0</v>
       </c>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="13"/>
-      <c r="T13" s="13"/>
-      <c r="U13" s="13"/>
-      <c r="V13" s="13"/>
       <c r="W13" s="13"/>
       <c r="X13" s="13"/>
       <c r="Y13" s="13"/>
@@ -14455,112 +14704,148 @@
       <c r="AB13" s="13"/>
       <c r="AC13" s="13"/>
       <c r="AD13" s="13"/>
+      <c r="AE13" s="13"/>
+      <c r="AF13" s="13"/>
+      <c r="AG13" s="13"/>
+      <c r="AH13" s="13"/>
+      <c r="AI13" s="13"/>
+      <c r="AJ13" s="13"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="7" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="15">
+        <v>29.0</v>
+      </c>
+      <c r="D14" s="15">
+        <v>16.0</v>
+      </c>
+      <c r="E14" s="15">
+        <v>0.64</v>
+      </c>
+      <c r="F14" s="15">
+        <v>109.0</v>
+      </c>
+      <c r="G14" s="15">
+        <v>78.0</v>
+      </c>
+      <c r="H14" s="15">
+        <v>0.58</v>
+      </c>
+      <c r="I14" s="7">
         <v>29.63</v>
       </c>
-      <c r="D14" s="14">
+      <c r="J14" s="14">
         <v>0.705</v>
       </c>
-      <c r="E14" s="7">
+      <c r="K14" s="7">
         <v>1.04</v>
       </c>
-      <c r="F14" s="7">
+      <c r="L14" s="7">
         <v>232.25</v>
       </c>
-      <c r="G14" s="7">
+      <c r="M14" s="7">
         <v>1.04</v>
       </c>
-      <c r="H14" s="14">
+      <c r="N14" s="14">
         <v>0.479</v>
       </c>
-      <c r="I14" s="7">
+      <c r="O14" s="7">
         <v>1.02</v>
       </c>
-      <c r="J14" s="7">
+      <c r="P14" s="7">
         <v>4.67</v>
       </c>
-      <c r="K14" s="7">
+      <c r="Q14" s="7">
         <v>0.11</v>
       </c>
-      <c r="L14" s="14">
+      <c r="R14" s="14">
         <v>0.574</v>
       </c>
-      <c r="M14" s="7">
+      <c r="S14" s="7">
         <v>1.06</v>
       </c>
-      <c r="N14" s="7">
+      <c r="T14" s="7">
         <v>2.31</v>
       </c>
-      <c r="O14" s="7">
+      <c r="U14" s="7">
         <v>0.5</v>
       </c>
-      <c r="P14" s="11">
+      <c r="V14" s="11">
         <v>2024.0</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="7" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="15">
+        <v>35.0</v>
+      </c>
+      <c r="D15" s="15">
+        <v>10.0</v>
+      </c>
+      <c r="E15" s="15">
+        <v>0.78</v>
+      </c>
+      <c r="F15" s="15">
+        <v>112.0</v>
+      </c>
+      <c r="G15" s="15">
+        <v>56.0</v>
+      </c>
+      <c r="H15" s="15">
+        <v>0.67</v>
+      </c>
+      <c r="I15" s="7">
         <v>28.07</v>
       </c>
-      <c r="D15" s="14">
+      <c r="J15" s="14">
         <v>0.702</v>
       </c>
-      <c r="E15" s="7">
+      <c r="K15" s="7">
         <v>1.07</v>
       </c>
-      <c r="F15" s="7">
+      <c r="L15" s="7">
         <v>229.64</v>
-      </c>
-      <c r="G15" s="7">
-        <v>1.05</v>
-      </c>
-      <c r="H15" s="14">
-        <v>0.587</v>
-      </c>
-      <c r="I15" s="7">
-        <v>1.01</v>
-      </c>
-      <c r="J15" s="7">
-        <v>4.79</v>
-      </c>
-      <c r="K15" s="7">
-        <v>0.63</v>
-      </c>
-      <c r="L15" s="14">
-        <v>0.679</v>
       </c>
       <c r="M15" s="7">
         <v>1.05</v>
       </c>
-      <c r="N15" s="7">
+      <c r="N15" s="14">
+        <v>0.587</v>
+      </c>
+      <c r="O15" s="7">
+        <v>1.01</v>
+      </c>
+      <c r="P15" s="7">
+        <v>4.79</v>
+      </c>
+      <c r="Q15" s="7">
+        <v>0.63</v>
+      </c>
+      <c r="R15" s="14">
+        <v>0.679</v>
+      </c>
+      <c r="S15" s="7">
+        <v>1.05</v>
+      </c>
+      <c r="T15" s="7">
         <v>2.4</v>
       </c>
-      <c r="O15" s="7">
+      <c r="U15" s="7">
         <v>0.6</v>
       </c>
-      <c r="P15" s="11">
+      <c r="V15" s="11">
         <v>2024.0</v>
       </c>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="13"/>
-      <c r="S15" s="13"/>
-      <c r="T15" s="13"/>
-      <c r="U15" s="13"/>
-      <c r="V15" s="13"/>
       <c r="W15" s="13"/>
       <c r="X15" s="13"/>
       <c r="Y15" s="13"/>
@@ -14569,112 +14854,148 @@
       <c r="AB15" s="13"/>
       <c r="AC15" s="13"/>
       <c r="AD15" s="13"/>
+      <c r="AE15" s="13"/>
+      <c r="AF15" s="13"/>
+      <c r="AG15" s="13"/>
+      <c r="AH15" s="13"/>
+      <c r="AI15" s="13"/>
+      <c r="AJ15" s="13"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="7" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="15">
+        <v>37.0</v>
+      </c>
+      <c r="D16" s="15">
+        <v>8.0</v>
+      </c>
+      <c r="E16" s="15">
+        <v>0.82</v>
+      </c>
+      <c r="F16" s="15">
+        <v>126.0</v>
+      </c>
+      <c r="G16" s="15">
+        <v>52.0</v>
+      </c>
+      <c r="H16" s="15">
+        <v>0.71</v>
+      </c>
+      <c r="I16" s="7">
         <v>22.87</v>
       </c>
-      <c r="D16" s="14">
+      <c r="J16" s="14">
         <v>0.69</v>
       </c>
-      <c r="E16" s="7">
+      <c r="K16" s="7">
         <v>1.1</v>
       </c>
-      <c r="F16" s="7">
+      <c r="L16" s="7">
         <v>231.48</v>
       </c>
-      <c r="G16" s="7">
+      <c r="M16" s="7">
         <v>1.12</v>
       </c>
-      <c r="H16" s="14">
+      <c r="N16" s="14">
         <v>0.657</v>
       </c>
-      <c r="I16" s="7">
+      <c r="O16" s="7">
         <v>1.14</v>
       </c>
-      <c r="J16" s="7">
+      <c r="P16" s="7">
         <v>5.09</v>
       </c>
-      <c r="K16" s="7">
+      <c r="Q16" s="7">
         <v>1.19</v>
       </c>
-      <c r="L16" s="14">
+      <c r="R16" s="14">
         <v>0.782</v>
       </c>
-      <c r="M16" s="7">
+      <c r="S16" s="7">
         <v>1.14</v>
       </c>
-      <c r="N16" s="7">
+      <c r="T16" s="7">
         <v>2.65</v>
       </c>
-      <c r="O16" s="7">
+      <c r="U16" s="7">
         <v>1.13</v>
       </c>
-      <c r="P16" s="11">
+      <c r="V16" s="11">
         <v>2024.0</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="7" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="15">
+        <v>30.0</v>
+      </c>
+      <c r="D17" s="15">
+        <v>16.0</v>
+      </c>
+      <c r="E17" s="15">
+        <v>0.65</v>
+      </c>
+      <c r="F17" s="15">
+        <v>108.0</v>
+      </c>
+      <c r="G17" s="15">
+        <v>76.0</v>
+      </c>
+      <c r="H17" s="15">
+        <v>0.59</v>
+      </c>
+      <c r="I17" s="7">
         <v>13.27</v>
       </c>
-      <c r="D17" s="14">
+      <c r="J17" s="14">
         <v>0.553</v>
       </c>
-      <c r="E17" s="7">
+      <c r="K17" s="7">
         <v>1.05</v>
       </c>
-      <c r="F17" s="7">
+      <c r="L17" s="7">
         <v>222.63</v>
       </c>
-      <c r="G17" s="7">
+      <c r="M17" s="7">
         <v>1.04</v>
       </c>
-      <c r="H17" s="14">
+      <c r="N17" s="14">
         <v>0.587</v>
       </c>
-      <c r="I17" s="7">
+      <c r="O17" s="7">
         <v>1.05</v>
       </c>
-      <c r="J17" s="7">
+      <c r="P17" s="7">
         <v>4.75</v>
       </c>
-      <c r="K17" s="7">
+      <c r="Q17" s="7">
         <v>0.39</v>
       </c>
-      <c r="L17" s="14">
+      <c r="R17" s="14">
         <v>0.561</v>
       </c>
-      <c r="M17" s="7">
+      <c r="S17" s="7">
         <v>1.03</v>
       </c>
-      <c r="N17" s="7">
+      <c r="T17" s="7">
         <v>2.21</v>
       </c>
-      <c r="O17" s="7">
+      <c r="U17" s="7">
         <v>0.3</v>
       </c>
-      <c r="P17" s="11">
+      <c r="V17" s="11">
         <v>2024.0</v>
       </c>
-      <c r="Q17" s="13"/>
-      <c r="R17" s="13"/>
-      <c r="S17" s="13"/>
-      <c r="T17" s="13"/>
-      <c r="U17" s="13"/>
-      <c r="V17" s="13"/>
       <c r="W17" s="13"/>
       <c r="X17" s="13"/>
       <c r="Y17" s="13"/>
@@ -14683,112 +15004,148 @@
       <c r="AB17" s="13"/>
       <c r="AC17" s="13"/>
       <c r="AD17" s="13"/>
+      <c r="AE17" s="13"/>
+      <c r="AF17" s="13"/>
+      <c r="AG17" s="13"/>
+      <c r="AH17" s="13"/>
+      <c r="AI17" s="13"/>
+      <c r="AJ17" s="13"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="7" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="15">
+        <v>16.0</v>
+      </c>
+      <c r="D18" s="15">
+        <v>24.0</v>
+      </c>
+      <c r="E18" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="F18" s="15">
+        <v>70.0</v>
+      </c>
+      <c r="G18" s="15">
+        <v>90.0</v>
+      </c>
+      <c r="H18" s="15">
+        <v>0.44</v>
+      </c>
+      <c r="I18" s="7">
         <v>2.38</v>
       </c>
-      <c r="D18" s="14">
+      <c r="J18" s="14">
         <v>0.508</v>
       </c>
-      <c r="E18" s="7">
+      <c r="K18" s="7">
         <v>1.05</v>
       </c>
-      <c r="F18" s="7">
+      <c r="L18" s="7">
         <v>218.89</v>
       </c>
-      <c r="G18" s="7">
+      <c r="M18" s="7">
         <v>1.02</v>
       </c>
-      <c r="H18" s="14">
+      <c r="N18" s="14">
         <v>0.346</v>
       </c>
-      <c r="I18" s="7">
+      <c r="O18" s="7">
         <v>0.96</v>
       </c>
-      <c r="J18" s="7">
+      <c r="P18" s="7">
         <v>4.21</v>
       </c>
-      <c r="K18" s="7">
+      <c r="Q18" s="7">
         <v>-0.69</v>
       </c>
-      <c r="L18" s="14">
+      <c r="R18" s="14">
         <v>0.475</v>
       </c>
-      <c r="M18" s="7">
+      <c r="S18" s="7">
         <v>1.01</v>
       </c>
-      <c r="N18" s="7">
+      <c r="T18" s="7">
         <v>1.93</v>
       </c>
-      <c r="O18" s="7">
+      <c r="U18" s="7">
         <v>-0.32</v>
       </c>
-      <c r="P18" s="11">
+      <c r="V18" s="11">
         <v>2024.0</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="7" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="15">
+        <v>11.0</v>
+      </c>
+      <c r="D19" s="15">
+        <v>25.0</v>
+      </c>
+      <c r="E19" s="15">
+        <v>0.31</v>
+      </c>
+      <c r="F19" s="15">
+        <v>56.0</v>
+      </c>
+      <c r="G19" s="15">
+        <v>90.0</v>
+      </c>
+      <c r="H19" s="15">
+        <v>0.38</v>
+      </c>
+      <c r="I19" s="7">
         <v>-5.59</v>
       </c>
-      <c r="D19" s="14">
+      <c r="J19" s="14">
         <v>0.443</v>
       </c>
-      <c r="E19" s="7">
+      <c r="K19" s="7">
         <v>0.94</v>
       </c>
-      <c r="F19" s="7">
+      <c r="L19" s="7">
         <v>213.38</v>
-      </c>
-      <c r="G19" s="7">
-        <v>0.95</v>
-      </c>
-      <c r="H19" s="14">
-        <v>0.55</v>
-      </c>
-      <c r="I19" s="7">
-        <v>0.99</v>
-      </c>
-      <c r="J19" s="7">
-        <v>4.68</v>
-      </c>
-      <c r="K19" s="7">
-        <v>0.12</v>
-      </c>
-      <c r="L19" s="14">
-        <v>0.326</v>
       </c>
       <c r="M19" s="7">
         <v>0.95</v>
       </c>
-      <c r="N19" s="7">
+      <c r="N19" s="14">
+        <v>0.55</v>
+      </c>
+      <c r="O19" s="7">
+        <v>0.99</v>
+      </c>
+      <c r="P19" s="7">
+        <v>4.68</v>
+      </c>
+      <c r="Q19" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="R19" s="14">
+        <v>0.326</v>
+      </c>
+      <c r="S19" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="T19" s="7">
         <v>1.7</v>
       </c>
-      <c r="O19" s="7">
+      <c r="U19" s="7">
         <v>-0.7</v>
       </c>
-      <c r="P19" s="11">
+      <c r="V19" s="11">
         <v>2024.0</v>
       </c>
-      <c r="Q19" s="13"/>
-      <c r="R19" s="13"/>
-      <c r="S19" s="13"/>
-      <c r="T19" s="13"/>
-      <c r="U19" s="13"/>
-      <c r="V19" s="13"/>
       <c r="W19" s="13"/>
       <c r="X19" s="13"/>
       <c r="Y19" s="13"/>
@@ -14797,112 +15154,148 @@
       <c r="AB19" s="13"/>
       <c r="AC19" s="13"/>
       <c r="AD19" s="13"/>
+      <c r="AE19" s="13"/>
+      <c r="AF19" s="13"/>
+      <c r="AG19" s="13"/>
+      <c r="AH19" s="13"/>
+      <c r="AI19" s="13"/>
+      <c r="AJ19" s="13"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="7" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="15">
+        <v>13.0</v>
+      </c>
+      <c r="D20" s="15">
+        <v>24.0</v>
+      </c>
+      <c r="E20" s="15">
+        <v>0.35</v>
+      </c>
+      <c r="F20" s="15">
+        <v>65.0</v>
+      </c>
+      <c r="G20" s="15">
+        <v>88.0</v>
+      </c>
+      <c r="H20" s="15">
+        <v>0.42</v>
+      </c>
+      <c r="I20" s="7">
         <v>-8.07</v>
       </c>
-      <c r="D20" s="14">
+      <c r="J20" s="14">
         <v>0.434</v>
       </c>
-      <c r="E20" s="7">
+      <c r="K20" s="7">
         <v>0.94</v>
       </c>
-      <c r="F20" s="7">
+      <c r="L20" s="7">
         <v>209.52</v>
-      </c>
-      <c r="G20" s="7">
-        <v>0.96</v>
-      </c>
-      <c r="H20" s="14">
-        <v>0.571</v>
-      </c>
-      <c r="I20" s="7">
-        <v>1.01</v>
-      </c>
-      <c r="J20" s="7">
-        <v>4.57</v>
-      </c>
-      <c r="K20" s="7">
-        <v>-0.02</v>
-      </c>
-      <c r="L20" s="14">
-        <v>0.438</v>
       </c>
       <c r="M20" s="7">
         <v>0.96</v>
       </c>
-      <c r="N20" s="7">
+      <c r="N20" s="14">
+        <v>0.571</v>
+      </c>
+      <c r="O20" s="7">
+        <v>1.01</v>
+      </c>
+      <c r="P20" s="7">
+        <v>4.57</v>
+      </c>
+      <c r="Q20" s="7">
+        <v>-0.02</v>
+      </c>
+      <c r="R20" s="14">
+        <v>0.438</v>
+      </c>
+      <c r="S20" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="T20" s="7">
         <v>2.1</v>
       </c>
-      <c r="O20" s="7">
+      <c r="U20" s="7">
         <v>-0.02</v>
       </c>
-      <c r="P20" s="11">
+      <c r="V20" s="11">
         <v>2024.0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="7" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="15">
+        <v>15.0</v>
+      </c>
+      <c r="D21" s="15">
+        <v>22.0</v>
+      </c>
+      <c r="E21" s="15">
+        <v>0.41</v>
+      </c>
+      <c r="F21" s="15">
+        <v>65.0</v>
+      </c>
+      <c r="G21" s="15">
+        <v>79.0</v>
+      </c>
+      <c r="H21" s="15">
+        <v>0.45</v>
+      </c>
+      <c r="I21" s="7">
         <v>-8.76</v>
       </c>
-      <c r="D21" s="14">
+      <c r="J21" s="14">
         <v>0.389</v>
       </c>
-      <c r="E21" s="7">
+      <c r="K21" s="7">
         <v>0.97</v>
       </c>
-      <c r="F21" s="7">
+      <c r="L21" s="7">
         <v>213.82</v>
       </c>
-      <c r="G21" s="7">
+      <c r="M21" s="7">
         <v>0.96</v>
       </c>
-      <c r="H21" s="14">
+      <c r="N21" s="14">
         <v>0.537</v>
       </c>
-      <c r="I21" s="7">
+      <c r="O21" s="7">
         <v>1.02</v>
       </c>
-      <c r="J21" s="7">
+      <c r="P21" s="7">
         <v>4.94</v>
       </c>
-      <c r="K21" s="7">
+      <c r="Q21" s="7">
         <v>0.24</v>
       </c>
-      <c r="L21" s="14">
+      <c r="R21" s="14">
         <v>0.386</v>
       </c>
-      <c r="M21" s="7">
+      <c r="S21" s="7">
         <v>0.91</v>
       </c>
-      <c r="N21" s="7">
+      <c r="T21" s="7">
         <v>1.66</v>
       </c>
-      <c r="O21" s="7">
+      <c r="U21" s="7">
         <v>-0.66</v>
       </c>
-      <c r="P21" s="11">
+      <c r="V21" s="11">
         <v>2024.0</v>
       </c>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13"/>
-      <c r="U21" s="13"/>
-      <c r="V21" s="13"/>
       <c r="W21" s="13"/>
       <c r="X21" s="13"/>
       <c r="Y21" s="13"/>
@@ -14911,112 +15304,148 @@
       <c r="AB21" s="13"/>
       <c r="AC21" s="13"/>
       <c r="AD21" s="13"/>
+      <c r="AE21" s="13"/>
+      <c r="AF21" s="13"/>
+      <c r="AG21" s="13"/>
+      <c r="AH21" s="13"/>
+      <c r="AI21" s="13"/>
+      <c r="AJ21" s="13"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="7" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="15">
+        <v>14.0</v>
+      </c>
+      <c r="D22" s="15">
+        <v>26.0</v>
+      </c>
+      <c r="E22" s="15">
+        <v>0.35</v>
+      </c>
+      <c r="F22" s="15">
+        <v>57.0</v>
+      </c>
+      <c r="G22" s="15">
+        <v>91.0</v>
+      </c>
+      <c r="H22" s="15">
+        <v>0.39</v>
+      </c>
+      <c r="I22" s="7">
         <v>-12.13</v>
       </c>
-      <c r="D22" s="14">
+      <c r="J22" s="14">
         <v>0.431</v>
       </c>
-      <c r="E22" s="7">
+      <c r="K22" s="7">
         <v>0.99</v>
       </c>
-      <c r="F22" s="7">
+      <c r="L22" s="7">
         <v>208.22</v>
       </c>
-      <c r="G22" s="7">
+      <c r="M22" s="7">
         <v>0.97</v>
       </c>
-      <c r="H22" s="14">
+      <c r="N22" s="14">
         <v>0.446</v>
       </c>
-      <c r="I22" s="7">
+      <c r="O22" s="7">
         <v>0.93</v>
       </c>
-      <c r="J22" s="7">
+      <c r="P22" s="7">
         <v>4.23</v>
       </c>
-      <c r="K22" s="7">
+      <c r="Q22" s="7">
         <v>-0.41</v>
       </c>
-      <c r="L22" s="14">
+      <c r="R22" s="14">
         <v>0.439</v>
       </c>
-      <c r="M22" s="7">
+      <c r="S22" s="7">
         <v>0.96</v>
       </c>
-      <c r="N22" s="7">
+      <c r="T22" s="7">
         <v>1.9</v>
       </c>
-      <c r="O22" s="7">
+      <c r="U22" s="7">
         <v>-0.15</v>
       </c>
-      <c r="P22" s="11">
+      <c r="V22" s="11">
         <v>2024.0</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="7" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="15">
+        <v>17.0</v>
+      </c>
+      <c r="D23" s="15">
+        <v>20.0</v>
+      </c>
+      <c r="E23" s="15">
+        <v>0.46</v>
+      </c>
+      <c r="F23" s="15">
+        <v>69.0</v>
+      </c>
+      <c r="G23" s="15">
+        <v>69.0</v>
+      </c>
+      <c r="H23" s="15">
+        <v>0.45</v>
+      </c>
+      <c r="I23" s="7">
         <v>-18.85</v>
       </c>
-      <c r="D23" s="14">
+      <c r="J23" s="14">
         <v>0.4</v>
       </c>
-      <c r="E23" s="7">
+      <c r="K23" s="7">
         <v>0.97</v>
       </c>
-      <c r="F23" s="7">
+      <c r="L23" s="7">
         <v>207.75</v>
       </c>
-      <c r="G23" s="7">
+      <c r="M23" s="7">
         <v>0.96</v>
       </c>
-      <c r="H23" s="14">
+      <c r="N23" s="14">
         <v>0.216</v>
       </c>
-      <c r="I23" s="7">
+      <c r="O23" s="7">
         <v>0.88</v>
       </c>
-      <c r="J23" s="7">
+      <c r="P23" s="7">
         <v>3.75</v>
       </c>
-      <c r="K23" s="7">
+      <c r="Q23" s="7">
         <v>-1.49</v>
       </c>
-      <c r="L23" s="14">
+      <c r="R23" s="14">
         <v>0.514</v>
       </c>
-      <c r="M23" s="7">
+      <c r="S23" s="7">
         <v>0.98</v>
       </c>
-      <c r="N23" s="7">
+      <c r="T23" s="7">
         <v>2.0</v>
       </c>
-      <c r="O23" s="7">
+      <c r="U23" s="7">
         <v>0.08</v>
       </c>
-      <c r="P23" s="11">
+      <c r="V23" s="11">
         <v>2024.0</v>
       </c>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="13"/>
-      <c r="T23" s="13"/>
-      <c r="U23" s="13"/>
-      <c r="V23" s="13"/>
       <c r="W23" s="13"/>
       <c r="X23" s="13"/>
       <c r="Y23" s="13"/>
@@ -15025,112 +15454,148 @@
       <c r="AB23" s="13"/>
       <c r="AC23" s="13"/>
       <c r="AD23" s="13"/>
+      <c r="AE23" s="13"/>
+      <c r="AF23" s="13"/>
+      <c r="AG23" s="13"/>
+      <c r="AH23" s="13"/>
+      <c r="AI23" s="13"/>
+      <c r="AJ23" s="13"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="7" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B24" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="15">
+        <v>6.0</v>
+      </c>
+      <c r="D24" s="15">
+        <v>27.0</v>
+      </c>
+      <c r="E24" s="15">
+        <v>0.18</v>
+      </c>
+      <c r="F24" s="15">
+        <v>47.0</v>
+      </c>
+      <c r="G24" s="15">
+        <v>87.0</v>
+      </c>
+      <c r="H24" s="15">
+        <v>0.35</v>
+      </c>
+      <c r="I24" s="7">
         <v>-19.98</v>
       </c>
-      <c r="D24" s="14">
+      <c r="J24" s="14">
         <v>0.328</v>
       </c>
-      <c r="E24" s="7">
+      <c r="K24" s="7">
         <v>0.92</v>
       </c>
-      <c r="F24" s="7">
+      <c r="L24" s="7">
         <v>206.75</v>
-      </c>
-      <c r="G24" s="7">
-        <v>0.93</v>
-      </c>
-      <c r="H24" s="14">
-        <v>0.462</v>
-      </c>
-      <c r="I24" s="7">
-        <v>0.95</v>
-      </c>
-      <c r="J24" s="7">
-        <v>4.29</v>
-      </c>
-      <c r="K24" s="7">
-        <v>-0.6</v>
-      </c>
-      <c r="L24" s="14">
-        <v>0.342</v>
       </c>
       <c r="M24" s="7">
         <v>0.93</v>
       </c>
-      <c r="N24" s="7">
+      <c r="N24" s="14">
+        <v>0.462</v>
+      </c>
+      <c r="O24" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="P24" s="7">
+        <v>4.29</v>
+      </c>
+      <c r="Q24" s="7">
+        <v>-0.6</v>
+      </c>
+      <c r="R24" s="14">
+        <v>0.342</v>
+      </c>
+      <c r="S24" s="7">
+        <v>0.93</v>
+      </c>
+      <c r="T24" s="7">
         <v>1.82</v>
       </c>
-      <c r="O24" s="7">
+      <c r="U24" s="7">
         <v>-0.63</v>
       </c>
-      <c r="P24" s="11">
+      <c r="V24" s="11">
         <v>2024.0</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="7" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="15">
+        <v>17.0</v>
+      </c>
+      <c r="D25" s="15">
+        <v>22.0</v>
+      </c>
+      <c r="E25" s="15">
+        <v>0.44</v>
+      </c>
+      <c r="F25" s="15">
+        <v>69.0</v>
+      </c>
+      <c r="G25" s="15">
+        <v>82.0</v>
+      </c>
+      <c r="H25" s="15">
+        <v>0.46</v>
+      </c>
+      <c r="I25" s="7">
         <v>-30.24</v>
       </c>
-      <c r="D25" s="14">
+      <c r="J25" s="14">
         <v>0.317</v>
       </c>
-      <c r="E25" s="7">
+      <c r="K25" s="7">
         <v>0.96</v>
       </c>
-      <c r="F25" s="7">
+      <c r="L25" s="7">
         <v>202.78</v>
       </c>
-      <c r="G25" s="7">
+      <c r="M25" s="7">
         <v>0.96</v>
       </c>
-      <c r="H25" s="14">
+      <c r="N25" s="14">
         <v>0.429</v>
       </c>
-      <c r="I25" s="7">
+      <c r="O25" s="7">
         <v>0.97</v>
       </c>
-      <c r="J25" s="7">
+      <c r="P25" s="7">
         <v>4.53</v>
       </c>
-      <c r="K25" s="7">
+      <c r="Q25" s="7">
         <v>-0.22</v>
       </c>
-      <c r="L25" s="14">
+      <c r="R25" s="14">
         <v>0.381</v>
       </c>
-      <c r="M25" s="7">
+      <c r="S25" s="7">
         <v>0.97</v>
       </c>
-      <c r="N25" s="7">
+      <c r="T25" s="7">
         <v>1.71</v>
       </c>
-      <c r="O25" s="7">
+      <c r="U25" s="7">
         <v>-0.6</v>
       </c>
-      <c r="P25" s="11">
+      <c r="V25" s="11">
         <v>2024.0</v>
       </c>
-      <c r="Q25" s="13"/>
-      <c r="R25" s="13"/>
-      <c r="S25" s="13"/>
-      <c r="T25" s="13"/>
-      <c r="U25" s="13"/>
-      <c r="V25" s="13"/>
       <c r="W25" s="13"/>
       <c r="X25" s="13"/>
       <c r="Y25" s="13"/>
@@ -15139,6 +15604,12 @@
       <c r="AB25" s="13"/>
       <c r="AC25" s="13"/>
       <c r="AD25" s="13"/>
+      <c r="AE25" s="13"/>
+      <c r="AF25" s="13"/>
+      <c r="AG25" s="13"/>
+      <c r="AH25" s="13"/>
+      <c r="AI25" s="13"/>
+      <c r="AJ25" s="13"/>
     </row>
     <row r="26" ht="15.75" customHeight="1"/>
     <row r="27" ht="15.75" customHeight="1"/>

</xml_diff>